<commit_message>
Dec20 - order object
</commit_message>
<xml_diff>
--- a/src/test/resources/Tdata.xlsx
+++ b/src/test/resources/Tdata.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.r\eclipse-workspace\CucumberFramework\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirut1500955\eclipse-workspace\TrailWork\.metadata\NewFork1QA\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5D7085-1AD7-49E0-9BD3-8100BF89EF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A8E268-0F48-40D9-8A76-3370D28816E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginPage" sheetId="2" r:id="rId2"/>
+    <sheet name="Order" sheetId="3" r:id="rId2"/>
+    <sheet name="LoginPage" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>AccountName</t>
   </si>
@@ -53,13 +54,61 @@
   </si>
   <si>
     <t>Automation@2024</t>
+  </si>
+  <si>
+    <t>TC_ID</t>
+  </si>
+  <si>
+    <t>ContractNumber</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>TC_001</t>
+  </si>
+  <si>
+    <t>Kevin Testing</t>
+  </si>
+  <si>
+    <t>00000101</t>
+  </si>
+  <si>
+    <t>Valid data</t>
+  </si>
+  <si>
+    <t>TC_002</t>
+  </si>
+  <si>
+    <t>Kirthy</t>
+  </si>
+  <si>
+    <t>333</t>
+  </si>
+  <si>
+    <t>Invalid data</t>
+  </si>
+  <si>
+    <t>TC_003</t>
+  </si>
+  <si>
+    <t>00000103</t>
+  </si>
+  <si>
+    <t>TC_004</t>
+  </si>
+  <si>
+    <t>Cathrine</t>
+  </si>
+  <si>
+    <t>00000102</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +120,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,10 +154,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -385,16 +445,16 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,7 +462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -417,21 +477,103 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C72C6DAC-49C3-4899-8096-E86BD6192FB1}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B9973C-C736-47F1-984F-C3ABF39B9667}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -442,7 +584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Asset Object Creation Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/Tdata.xlsx
+++ b/src/test/resources/Tdata.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.r\eclipse-workspace\CucumberFramework\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gobin1500842\git\QA_Automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5D7085-1AD7-49E0-9BD3-8100BF89EF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8E1908-B19C-48D3-82A4-D4A663CDE3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginPage" sheetId="2" r:id="rId2"/>
+    <sheet name="Asset" sheetId="3" r:id="rId2"/>
+    <sheet name="LoginPage" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>AccountName</t>
   </si>
@@ -53,6 +54,18 @@
   </si>
   <si>
     <t>Automation@2024</t>
+  </si>
+  <si>
+    <t>AssetName</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>test asset name</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -385,7 +398,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -417,10 +430,51 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A632D6E2-5CF1-4C26-8928-458BB8A53AFB}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B9973C-C736-47F1-984F-C3ABF39B9667}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Opportunity and Quote commit
</commit_message>
<xml_diff>
--- a/src/test/resources/Tdata.xlsx
+++ b/src/test/resources/Tdata.xlsx
@@ -5,21 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vigne1500998\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abina1501006\Automation Projects\folder1\QA_Automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F873FD0-4C49-4D31-8276-371F674F69C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C77C42-FA85-4F2B-BC5F-9AD46AFFE273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Order" sheetId="3" r:id="rId1"/>
-    <sheet name="Campaign" sheetId="5" r:id="rId2"/>
-    <sheet name="Account" sheetId="6" r:id="rId3"/>
-    <sheet name="Contact" sheetId="7" r:id="rId4"/>
-    <sheet name="Asset" sheetId="4" r:id="rId5"/>
-    <sheet name="Contract" sheetId="1" r:id="rId6"/>
-    <sheet name="LoginPage" sheetId="2" r:id="rId7"/>
+    <sheet name="LoginPage" sheetId="2" r:id="rId1"/>
+    <sheet name="Order" sheetId="3" r:id="rId2"/>
+    <sheet name="Campaign" sheetId="5" r:id="rId3"/>
+    <sheet name="Account" sheetId="6" r:id="rId4"/>
+    <sheet name="Contact" sheetId="7" r:id="rId5"/>
+    <sheet name="Asset" sheetId="4" r:id="rId6"/>
+    <sheet name="Opportunity" sheetId="8" r:id="rId7"/>
+    <sheet name="Quote" sheetId="9" r:id="rId8"/>
+    <sheet name="Contract" sheetId="1" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>AccountName</t>
   </si>
@@ -57,181 +59,202 @@
     <t>qateam@automation.com</t>
   </si>
   <si>
+    <t>TC_ID</t>
+  </si>
+  <si>
+    <t>ContractNumber</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>TC_001</t>
+  </si>
+  <si>
+    <t>Kevin Testing</t>
+  </si>
+  <si>
+    <t>00000101</t>
+  </si>
+  <si>
+    <t>Valid data</t>
+  </si>
+  <si>
+    <t>TC_002</t>
+  </si>
+  <si>
+    <t>Kirthy</t>
+  </si>
+  <si>
+    <t>333</t>
+  </si>
+  <si>
+    <t>Invalid data</t>
+  </si>
+  <si>
+    <t>TC_003</t>
+  </si>
+  <si>
+    <t>00000103</t>
+  </si>
+  <si>
+    <t>TC_004</t>
+  </si>
+  <si>
+    <t>Cathrine</t>
+  </si>
+  <si>
+    <t>00000102</t>
+  </si>
+  <si>
+    <t>AssetName</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>Test Asset QA</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>CampaignName</t>
+  </si>
+  <si>
+    <t>Campaign QA</t>
+  </si>
+  <si>
+    <t>Account name</t>
+  </si>
+  <si>
+    <t>Acc number</t>
+  </si>
+  <si>
+    <t>Accountsite</t>
+  </si>
+  <si>
+    <t>Acc Type</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Annualrevenue</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Tickersymbol</t>
+  </si>
+  <si>
+    <t>Employees</t>
+  </si>
+  <si>
+    <t>SICcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description </t>
+  </si>
+  <si>
+    <t>Account excel input</t>
+  </si>
+  <si>
+    <t>testSite</t>
+  </si>
+  <si>
+    <t>Prospect</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>Hot</t>
+  </si>
+  <si>
+    <t>testFax</t>
+  </si>
+  <si>
+    <t>salesforce.com</t>
+  </si>
+  <si>
+    <t>testTickersymbol</t>
+  </si>
+  <si>
+    <t>Automation implementation testing</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Account Name</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Vignesh</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Vignesh Testing</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Opportunity Name</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>My Opportunity</t>
+  </si>
+  <si>
+    <t>Prospecting</t>
+  </si>
+  <si>
+    <t>Quotename</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>My Quote</t>
+  </si>
+  <si>
+    <t>quote</t>
+  </si>
+  <si>
     <t>Automation@2024</t>
   </si>
   <si>
-    <t>TC_ID</t>
-  </si>
-  <si>
-    <t>ContractNumber</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>TC_001</t>
-  </si>
-  <si>
-    <t>Kevin Testing</t>
-  </si>
-  <si>
-    <t>00000101</t>
-  </si>
-  <si>
-    <t>Valid data</t>
-  </si>
-  <si>
-    <t>TC_002</t>
-  </si>
-  <si>
-    <t>Kirthy</t>
-  </si>
-  <si>
-    <t>333</t>
-  </si>
-  <si>
-    <t>Invalid data</t>
-  </si>
-  <si>
-    <t>TC_003</t>
-  </si>
-  <si>
-    <t>00000103</t>
-  </si>
-  <si>
-    <t>TC_004</t>
-  </si>
-  <si>
-    <t>Cathrine</t>
-  </si>
-  <si>
-    <t>00000102</t>
-  </si>
-  <si>
-    <t>AssetName</t>
-  </si>
-  <si>
-    <t>ContactName</t>
-  </si>
-  <si>
-    <t>Test Asset QA</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>CampaignName</t>
-  </si>
-  <si>
-    <t>Campaign QA</t>
-  </si>
-  <si>
-    <t>Account name</t>
-  </si>
-  <si>
-    <t>Acc number</t>
-  </si>
-  <si>
-    <t>Accountsite</t>
-  </si>
-  <si>
-    <t>Acc Type</t>
-  </si>
-  <si>
-    <t>Industry</t>
-  </si>
-  <si>
-    <t>Annualrevenue</t>
-  </si>
-  <si>
-    <t>Rating</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Fax</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
-    <t>Tickersymbol</t>
-  </si>
-  <si>
-    <t>Employees</t>
-  </si>
-  <si>
-    <t>SICcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description </t>
-  </si>
-  <si>
-    <t>Account excel input</t>
-  </si>
-  <si>
-    <t>testSite</t>
-  </si>
-  <si>
-    <t>Prospect</t>
-  </si>
-  <si>
-    <t>Agriculture</t>
-  </si>
-  <si>
-    <t>Hot</t>
-  </si>
-  <si>
-    <t>testFax</t>
-  </si>
-  <si>
-    <t>salesforce.com</t>
-  </si>
-  <si>
-    <t>testTickersymbol</t>
-  </si>
-  <si>
-    <t>Automation implementation testing</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>8975461236</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Account Name</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Vignesh</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Vignesh Testing</t>
-  </si>
-  <si>
-    <t>Automation</t>
+    <t>Expiration Date</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>quote@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -302,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -318,6 +341,19 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -598,11 +634,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B9973C-C736-47F1-984F-C3ABF39B9667}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{B22C74DF-FAB0-4BE2-B86E-2B1F05AEE0FF}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{38CBCE21-E102-4A84-B94C-D8909BC79172}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{77B6A4DE-3A85-4F5E-BCFD-0CF6D1E4F60D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDE2E92-4439-43EA-9EB0-C95AD66E8DA3}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,69 +698,69 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" t="s">
         <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -685,7 +768,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16FC4A38-509A-487B-BE8B-40570D5F46F0}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -700,13 +783,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -715,12 +798,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7539949-F6C4-4D9A-89DD-8CBA43A98500}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,108 +811,129 @@
     <col min="1" max="1" width="28.109375" customWidth="1"/>
     <col min="2" max="2" width="30.21875" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" customWidth="1"/>
     <col min="11" max="11" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2">
+        <v>50000</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="10">
+        <v>8975461236</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2">
         <v>55</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" s="5" t="s">
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>53</v>
-      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="6"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFADF833-7B24-4523-B982-3AA73E12501C}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
@@ -837,70 +941,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50263DD-6049-4357-BFFE-76AA00E30E47}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -909,11 +973,207 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50263DD-6049-4357-BFFE-76AA00E30E47}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13C5E886-964C-460F-A0C1-419120F7A3E1}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67B5F94-95D4-486A-8CF5-CDB0D037011E}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="22.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="11">
+        <v>45328</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2" s="9">
+        <v>9876543210</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{0E6E189E-DD25-4C23-8ADE-9A1FB1304E45}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -942,51 +1202,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B9973C-C736-47F1-984F-C3ABF39B9667}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{B22C74DF-FAB0-4BE2-B86E-2B1F05AEE0FF}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{38CBCE21-E102-4A84-B94C-D8909BC79172}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{C152FB5F-3DAA-4CB4-90C1-1D0C50E92A4C}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Contract & Order - Update/ Delete scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/Tdata.xlsx
+++ b/src/test/resources/Tdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abina1501006\Automation Projects\folder1\QA_Automation\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie1500956\git\QA_Automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C77C42-FA85-4F2B-BC5F-9AD46AFFE273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D87C842-78AA-42ED-9035-0DFBD9FEEA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="78">
   <si>
     <t>AccountName</t>
   </si>
@@ -245,9 +245,6 @@
     <t>quote</t>
   </si>
   <si>
-    <t>Automation@2024</t>
-  </si>
-  <si>
     <t>Expiration Date</t>
   </si>
   <si>
@@ -255,6 +252,21 @@
   </si>
   <si>
     <t>quote@yopmail.com</t>
+  </si>
+  <si>
+    <t>ContractTermUpdated</t>
+  </si>
+  <si>
+    <t>UpdateAccountName</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>Test brook street</t>
+  </si>
+  <si>
+    <t>Automation@March24</t>
   </si>
 </sst>
 </file>
@@ -637,18 +649,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B9973C-C736-47F1-984F-C3ABF39B9667}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -659,7 +671,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -667,7 +679,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -682,21 +694,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDE2E92-4439-43EA-9EB0-C95AD66E8DA3}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -709,8 +722,11 @@
       <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -723,8 +739,11 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -738,7 +757,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -749,7 +768,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -776,18 +795,18 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -806,21 +825,21 @@
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.109375" customWidth="1"/>
-    <col min="2" max="2" width="30.21875" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="23.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" customWidth="1"/>
-    <col min="10" max="10" width="19.109375" customWidth="1"/>
-    <col min="11" max="11" width="36.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.08984375" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="22.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="23.54296875" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" customWidth="1"/>
+    <col min="10" max="10" width="19.08984375" customWidth="1"/>
+    <col min="11" max="11" width="36.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
@@ -864,7 +883,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>44</v>
       </c>
@@ -908,7 +927,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
@@ -937,9 +956,9 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -953,7 +972,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -980,13 +999,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -997,7 +1016,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1018,16 +1037,16 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -1035,7 +1054,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -1053,23 +1072,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67B5F94-95D4-486A-8CF5-CDB0D037011E}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="22.21875" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="27.109375" customWidth="1"/>
+    <col min="1" max="2" width="22.1796875" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" customWidth="1"/>
+    <col min="5" max="5" width="27.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>66</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>67</v>
@@ -1078,14 +1097,14 @@
         <v>37</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>38</v>
       </c>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>68</v>
       </c>
@@ -1099,14 +1118,14 @@
         <v>9876543210</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>69</v>
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1115,7 +1134,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1124,7 +1143,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1133,7 +1152,7 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1142,7 +1161,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1151,7 +1170,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1170,32 +1189,46 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes of Asset Page detail along with highlighter. Also updated the test data file to select the lookup of contact name.
</commit_message>
<xml_diff>
--- a/src/test/resources/Tdata.xlsx
+++ b/src/test/resources/Tdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie1500956\git\QA_Automation\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gobin1500842\git\QA_Automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D87C842-78AA-42ED-9035-0DFBD9FEEA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149CD13C-E510-4251-9C88-24A0329A7510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
   <si>
     <t>AccountName</t>
   </si>
@@ -113,18 +113,9 @@
     <t>ContactName</t>
   </si>
   <si>
-    <t>Test Asset QA</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>CampaignName</t>
   </si>
   <si>
-    <t>Campaign QA</t>
-  </si>
-  <si>
     <t>Account name</t>
   </si>
   <si>
@@ -167,9 +158,6 @@
     <t xml:space="preserve">Description </t>
   </si>
   <si>
-    <t>Account excel input</t>
-  </si>
-  <si>
     <t>testSite</t>
   </si>
   <si>
@@ -209,15 +197,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Vignesh</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Vignesh Testing</t>
-  </si>
-  <si>
     <t>Automation</t>
   </si>
   <si>
@@ -227,9 +206,6 @@
     <t>Stage</t>
   </si>
   <si>
-    <t>My Opportunity</t>
-  </si>
-  <si>
     <t>Prospecting</t>
   </si>
   <si>
@@ -239,9 +215,6 @@
     <t>Tax</t>
   </si>
   <si>
-    <t>My Quote</t>
-  </si>
-  <si>
     <t>quote</t>
   </si>
   <si>
@@ -267,6 +240,39 @@
   </si>
   <si>
     <t>Automation@March24</t>
+  </si>
+  <si>
+    <t>Test Asset Contact</t>
+  </si>
+  <si>
+    <t>Test Asset Account</t>
+  </si>
+  <si>
+    <t>Test QA Asset</t>
+  </si>
+  <si>
+    <t>UpdatedAssetName</t>
+  </si>
+  <si>
+    <t>Test QA Asset Updated</t>
+  </si>
+  <si>
+    <t>Test Campaign QA</t>
+  </si>
+  <si>
+    <t>Test Account excel input</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Test QA</t>
+  </si>
+  <si>
+    <t>Test My Opportunity</t>
+  </si>
+  <si>
+    <t>Test My Quote</t>
   </si>
 </sst>
 </file>
@@ -649,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B9973C-C736-47F1-984F-C3ABF39B9667}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -679,7 +685,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -723,7 +729,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -740,7 +746,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -792,7 +798,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -802,13 +808,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -821,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7539949-F6C4-4D9A-89DD-8CBA43A98500}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -841,81 +847,81 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="K1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F2">
         <v>50000</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H2" s="10">
         <v>8975461236</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L2">
         <v>55</v>
@@ -924,7 +930,7 @@
         <v>2</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -953,37 +959,42 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -993,19 +1004,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50263DD-6049-4357-BFFE-76AA00E30E47}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.08984375" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1015,16 +1028,22 @@
       <c r="C1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1037,7 +1056,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1048,18 +1067,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C2" s="13"/>
     </row>
@@ -1073,7 +1092,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1085,28 +1104,28 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B2" s="11">
         <v>45328</v>
@@ -1118,10 +1137,10 @@
         <v>9876543210</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G2" s="5"/>
     </row>
@@ -1191,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1211,10 +1230,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>